<commit_message>
fix: testcases fixed w.r.t adjustTick change
</commit_message>
<xml_diff>
--- a/test/scenarios/Deposit_Test.xlsx
+++ b/test/scenarios/Deposit_Test.xlsx
@@ -423,54 +423,108 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -479,60 +533,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1696,818 +1696,818 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="19.95" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="24.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="39.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="39.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="25" width="16.33203125" style="2" customWidth="1"/>
-    <col min="26" max="16384" width="16.33203125" style="2"/>
+    <col min="1" max="1" width="20.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="24.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="39.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="39.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="25" width="16.33203125" style="1" customWidth="1"/>
+    <col min="26" max="16384" width="16.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="27.6" customHeight="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34"/>
+      <c r="S1" s="34"/>
+      <c r="T1" s="34"/>
+      <c r="U1" s="34"/>
+      <c r="V1" s="34"/>
+      <c r="W1" s="34"/>
+      <c r="X1" s="34"/>
     </row>
     <row r="2" spans="1:24" ht="20.85" customHeight="1">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7"/>
-      <c r="W2" s="7"/>
-      <c r="X2" s="7"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
     </row>
     <row r="3" spans="1:24" ht="20.100000000000001" customHeight="1">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
-      <c r="V3" s="7"/>
-      <c r="W3" s="7"/>
-      <c r="X3" s="7"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
     </row>
     <row r="4" spans="1:24" ht="20.85" customHeight="1">
-      <c r="A4" s="10">
+      <c r="A4" s="7">
         <v>1</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="8">
         <v>3060.095307</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
-      <c r="T4" s="7"/>
-      <c r="U4" s="7"/>
-      <c r="V4" s="7"/>
-      <c r="W4" s="7"/>
-      <c r="X4" s="7"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
     </row>
     <row r="5" spans="1:24" ht="21.75" customHeight="1">
-      <c r="A5" s="14"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="17" t="s">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="17" t="s">
+      <c r="E5" s="36"/>
+      <c r="F5" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="17" t="s">
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="N5" s="19"/>
-      <c r="O5" s="18"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
-      <c r="W5" s="7"/>
-      <c r="X5" s="7"/>
+      <c r="N5" s="37"/>
+      <c r="O5" s="36"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
     </row>
     <row r="6" spans="1:24" ht="20.85" customHeight="1">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="24" t="s">
+      <c r="B6" s="30"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="25" t="s">
+      <c r="G6" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="25" t="s">
+      <c r="H6" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="25" t="s">
+      <c r="I6" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="25" t="s">
+      <c r="J6" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="25" t="s">
+      <c r="K6" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="L6" s="25" t="s">
+      <c r="L6" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="M6" s="25" t="s">
+      <c r="M6" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="N6" s="25" t="s">
+      <c r="N6" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="O6" s="26" t="s">
+      <c r="O6" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7"/>
-      <c r="U6" s="7"/>
-      <c r="V6" s="7"/>
-      <c r="W6" s="7"/>
-      <c r="X6" s="7"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+      <c r="W6" s="4"/>
+      <c r="X6" s="4"/>
     </row>
     <row r="7" spans="1:24" ht="20.85" customHeight="1">
-      <c r="A7" s="27"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="10">
+      <c r="A7" s="31"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="7">
         <v>1</v>
       </c>
-      <c r="E7" s="28">
+      <c r="E7" s="19">
         <v>4000</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F7" s="19">
         <f>O7</f>
         <v>1E+18</v>
       </c>
-      <c r="G7" s="28">
+      <c r="G7" s="19">
         <v>0</v>
       </c>
-      <c r="H7" s="28">
+      <c r="H7" s="19">
         <v>0</v>
       </c>
-      <c r="I7" s="28">
+      <c r="I7" s="19">
         <f>M7</f>
         <v>1</v>
       </c>
-      <c r="J7" s="28">
+      <c r="J7" s="19">
         <f>N7</f>
         <v>3060.095307</v>
       </c>
-      <c r="K7" s="28">
+      <c r="K7" s="19">
         <f>IF(G7&gt;0,G7*0.01,0)</f>
         <v>0</v>
       </c>
-      <c r="L7" s="28">
+      <c r="L7" s="19">
         <f>IF(H7&gt;0,H7*0.01,0)</f>
         <v>0</v>
       </c>
-      <c r="M7" s="28">
+      <c r="M7" s="19">
         <f>MIN(D7,E8)</f>
         <v>1</v>
       </c>
-      <c r="N7" s="28">
+      <c r="N7" s="19">
         <f>MIN(E7,D8)</f>
         <v>3060.095307</v>
       </c>
-      <c r="O7" s="11">
+      <c r="O7" s="8">
         <f>MAX(M7*1000000000000000000,N7*1000000)</f>
         <v>1E+18</v>
       </c>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="7"/>
-      <c r="U7" s="7"/>
-      <c r="V7" s="7"/>
-      <c r="W7" s="7"/>
-      <c r="X7" s="7"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+      <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
     </row>
     <row r="8" spans="1:24" ht="20.85" customHeight="1">
-      <c r="A8" s="29"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="32">
+      <c r="A8" s="20"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="23">
         <f>IF($B4&gt;$A4,D7*$B4,D7/$A4)</f>
         <v>3060.095307</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="23">
         <f>IF($B4=1,E7*$A4,E7/$B4)</f>
         <v>1.3071488299236818</v>
       </c>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="33"/>
-      <c r="N8" s="33"/>
-      <c r="O8" s="33"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="6"/>
-      <c r="U8" s="6"/>
-      <c r="V8" s="6"/>
-      <c r="W8" s="6"/>
-      <c r="X8" s="6"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="24"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
     </row>
     <row r="9" spans="1:24" ht="20.85" customHeight="1">
-      <c r="A9" s="29"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="6"/>
-      <c r="S9" s="6"/>
-      <c r="T9" s="6"/>
-      <c r="U9" s="6"/>
-      <c r="V9" s="6"/>
-      <c r="W9" s="6"/>
-      <c r="X9" s="6"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
     </row>
     <row r="10" spans="1:24" ht="20.85" customHeight="1">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="24" t="s">
+      <c r="B10" s="30"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="25" t="s">
+      <c r="F10" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="25" t="s">
+      <c r="G10" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="25" t="s">
+      <c r="H10" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="25" t="s">
+      <c r="I10" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="J10" s="25" t="s">
+      <c r="J10" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="K10" s="25" t="s">
+      <c r="K10" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="L10" s="25" t="s">
+      <c r="L10" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="M10" s="25" t="s">
+      <c r="M10" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="N10" s="25" t="s">
+      <c r="N10" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="O10" s="26" t="s">
+      <c r="O10" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
-      <c r="S10" s="7"/>
-      <c r="T10" s="7"/>
-      <c r="U10" s="7"/>
-      <c r="V10" s="7"/>
-      <c r="W10" s="7"/>
-      <c r="X10" s="7"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="4"/>
+      <c r="X10" s="4"/>
     </row>
     <row r="11" spans="1:24" ht="20.85" customHeight="1">
-      <c r="A11" s="27"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="10">
+      <c r="A11" s="31"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="7">
         <v>10</v>
       </c>
-      <c r="E11" s="28">
+      <c r="E11" s="19">
         <v>5000</v>
       </c>
-      <c r="F11" s="28">
+      <c r="F11" s="19">
         <f>F7+O11</f>
         <v>2.6339360374046024E+18</v>
       </c>
-      <c r="G11" s="28">
+      <c r="G11" s="19">
         <v>0</v>
       </c>
-      <c r="H11" s="28">
+      <c r="H11" s="19">
         <v>0</v>
       </c>
-      <c r="I11" s="28">
+      <c r="I11" s="19">
         <f>I7+M11</f>
         <v>2.6339360374046024</v>
       </c>
-      <c r="J11" s="28">
+      <c r="J11" s="19">
         <f>J7+N11</f>
         <v>8060.0953069999996</v>
       </c>
-      <c r="K11" s="28">
+      <c r="K11" s="19">
         <f>IF(G11&gt;0,G11*0.01,0)</f>
         <v>0</v>
       </c>
-      <c r="L11" s="28">
+      <c r="L11" s="19">
         <f>IF(H11&gt;0,H11*0.01,0)</f>
         <v>0</v>
       </c>
-      <c r="M11" s="28">
+      <c r="M11" s="19">
         <f>MIN(D11,E12)</f>
         <v>1.6339360374046024</v>
       </c>
-      <c r="N11" s="28">
+      <c r="N11" s="19">
         <f>MIN(E11,D12)</f>
         <v>5000</v>
       </c>
-      <c r="O11" s="11">
+      <c r="O11" s="8">
         <f>MAX(M11*1000000000000000000,N11*1000000)</f>
         <v>1.6339360374046024E+18</v>
       </c>
-      <c r="P11" s="21"/>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="7"/>
-      <c r="S11" s="7"/>
-      <c r="T11" s="7"/>
-      <c r="U11" s="7"/>
-      <c r="V11" s="7"/>
-      <c r="W11" s="7"/>
-      <c r="X11" s="7"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="4"/>
+      <c r="W11" s="4"/>
+      <c r="X11" s="4"/>
     </row>
     <row r="12" spans="1:24" ht="20.85" customHeight="1">
-      <c r="A12" s="7"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="32">
+      <c r="A12" s="4"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="23">
         <f>IF($B4&gt;$A4,D11*$B4,D11/$A4)</f>
         <v>30600.95307</v>
       </c>
-      <c r="E12" s="32">
+      <c r="E12" s="23">
         <f>IF($B4=1,E11*$A4,E11/$B4)</f>
         <v>1.6339360374046024</v>
       </c>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
-      <c r="S12" s="7"/>
-      <c r="T12" s="7"/>
-      <c r="U12" s="7"/>
-      <c r="V12" s="7"/>
-      <c r="W12" s="7"/>
-      <c r="X12" s="7"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="4"/>
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
     </row>
     <row r="13" spans="1:24" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="7"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="7"/>
-      <c r="S13" s="7"/>
-      <c r="T13" s="7"/>
-      <c r="U13" s="7"/>
-      <c r="V13" s="7"/>
-      <c r="W13" s="7"/>
-      <c r="X13" s="7"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="4"/>
+      <c r="W13" s="4"/>
+      <c r="X13" s="4"/>
     </row>
     <row r="14" spans="1:24" ht="20.85" customHeight="1">
-      <c r="A14" s="7"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="35">
+      <c r="A14" s="4"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="26">
         <f>F11</f>
         <v>2.6339360374046024E+18</v>
       </c>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="35">
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="26">
         <f>IF($G$16&gt;0,($I$11+$G$16)-($G$16*0.01),$I$11+$G$16)</f>
-        <v>2.6369673616171299</v>
-      </c>
-      <c r="J14" s="35">
+        <v>2.6369764676447822</v>
+      </c>
+      <c r="J14" s="26">
         <f>IF($H$16&gt;0,$J$11+$H$16-($H$16*0.01),$J$11+$H$16)</f>
-        <v>12180.64601765</v>
-      </c>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="7"/>
-      <c r="R14" s="7"/>
-      <c r="S14" s="7"/>
-      <c r="T14" s="7"/>
-      <c r="U14" s="7"/>
-      <c r="V14" s="7"/>
-      <c r="W14" s="7"/>
-      <c r="X14" s="7"/>
+        <v>12168.303505490001</v>
+      </c>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="4"/>
+      <c r="W14" s="4"/>
+      <c r="X14" s="4"/>
     </row>
     <row r="15" spans="1:24" ht="20.85" customHeight="1">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="24" t="s">
+      <c r="B15" s="30"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="25" t="s">
+      <c r="F15" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="25" t="s">
+      <c r="G15" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="25" t="s">
+      <c r="H15" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I15" s="25" t="s">
+      <c r="I15" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="J15" s="25" t="s">
+      <c r="J15" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="K15" s="25" t="s">
+      <c r="K15" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="L15" s="25" t="s">
+      <c r="L15" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="M15" s="25" t="s">
+      <c r="M15" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="N15" s="25" t="s">
+      <c r="N15" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="O15" s="26" t="s">
+      <c r="O15" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="P15" s="21"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="7"/>
-      <c r="T15" s="7"/>
-      <c r="U15" s="7"/>
-      <c r="V15" s="7"/>
-      <c r="W15" s="7"/>
-      <c r="X15" s="7"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+      <c r="U15" s="4"/>
+      <c r="V15" s="4"/>
+      <c r="W15" s="4"/>
+      <c r="X15" s="4"/>
     </row>
     <row r="16" spans="1:24" ht="20.85" customHeight="1">
-      <c r="A16" s="27"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="10">
+      <c r="A16" s="31"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="7">
         <v>10</v>
       </c>
-      <c r="E16" s="28">
+      <c r="E16" s="19">
         <v>8000</v>
       </c>
-      <c r="F16" s="28">
+      <c r="F16" s="19">
         <f>F14+O16</f>
-        <v>4.363851533569897E+18</v>
-      </c>
-      <c r="G16" s="28">
+        <v>4.3656062155629583E+18</v>
+      </c>
+      <c r="G16" s="19">
         <f>G21-I11</f>
-        <v>3.0619436490177954E-3</v>
-      </c>
-      <c r="H16" s="28">
+        <v>3.0711416567474892E-3</v>
+      </c>
+      <c r="H16" s="19">
         <f>H21-J11</f>
-        <v>4162.1724350000004</v>
-      </c>
-      <c r="I16" s="28">
+        <v>4149.7052510000012</v>
+      </c>
+      <c r="I16" s="19">
         <f>I14+M16</f>
-        <v>4.3688737697311897</v>
-      </c>
-      <c r="J16" s="28">
+        <v>4.3706455638138761</v>
+      </c>
+      <c r="J16" s="19">
         <f>J14+N16</f>
-        <v>20180.64601765</v>
-      </c>
-      <c r="K16" s="28">
+        <v>20168.303505490003</v>
+      </c>
+      <c r="K16" s="19">
         <f>IF(G16&gt;0,G16*0.01,0)</f>
-        <v>3.0619436490177952E-5</v>
-      </c>
-      <c r="L16" s="28">
+        <v>3.0711416567474889E-5</v>
+      </c>
+      <c r="L16" s="19">
         <f>IF(H16&gt;0,H16*0.01,0)</f>
-        <v>41.621724350000008</v>
-      </c>
-      <c r="M16" s="28">
+        <v>41.49705251000001</v>
+      </c>
+      <c r="M16" s="19">
         <f>MIN(D16,E17)</f>
-        <v>1.7319064081140596</v>
-      </c>
-      <c r="N16" s="28">
+        <v>1.7336690961690941</v>
+      </c>
+      <c r="N16" s="19">
         <f>MIN(E16,D17)</f>
         <v>8000</v>
       </c>
-      <c r="O16" s="11">
+      <c r="O16" s="8">
         <f>IF($B$4&gt;$A$4,N16*F17,M16*F17)</f>
-        <v>1.7299154961652946E+18</v>
-      </c>
-      <c r="P16" s="21"/>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="7"/>
-      <c r="S16" s="7"/>
-      <c r="T16" s="7"/>
-      <c r="U16" s="7"/>
-      <c r="V16" s="7"/>
-      <c r="W16" s="7"/>
-      <c r="X16" s="7"/>
+        <v>1.731670178158356E+18</v>
+      </c>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+      <c r="U16" s="4"/>
+      <c r="V16" s="4"/>
+      <c r="W16" s="4"/>
+      <c r="X16" s="4"/>
     </row>
     <row r="17" spans="1:24" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A17" s="13"/>
-      <c r="B17" s="36"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="32">
+      <c r="A17" s="10"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="23">
         <f>IF($B20&gt;$A20,D16*$B20,D16/$A20)</f>
-        <v>46191.872508350563</v>
-      </c>
-      <c r="E17" s="32">
+        <v>46144.907454817527</v>
+      </c>
+      <c r="E17" s="23">
         <f>IF($B20=1,E16*$A20,E16/$B20)</f>
-        <v>1.7319064081140596</v>
-      </c>
-      <c r="F17" s="32">
+        <v>1.7336690961690941</v>
+      </c>
+      <c r="F17" s="23">
         <f>IF(J14&gt;0,IF($B4&gt;$A4,F14/J14,F14/I14),0)</f>
-        <v>216239437020661.81</v>
-      </c>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
-      <c r="K17" s="33"/>
-      <c r="L17" s="33"/>
-      <c r="M17" s="33"/>
-      <c r="N17" s="33"/>
-      <c r="O17" s="33"/>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="7"/>
-      <c r="S17" s="7"/>
-      <c r="T17" s="7"/>
-      <c r="U17" s="7"/>
-      <c r="V17" s="7"/>
-      <c r="W17" s="7"/>
-      <c r="X17" s="7"/>
+        <v>216458772269794.5</v>
+      </c>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="24"/>
+      <c r="N17" s="24"/>
+      <c r="O17" s="24"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+      <c r="U17" s="4"/>
+      <c r="V17" s="4"/>
+      <c r="W17" s="4"/>
+      <c r="X17" s="4"/>
     </row>
     <row r="18" spans="1:24" ht="32.85" customHeight="1">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
-      <c r="Q18" s="7"/>
-      <c r="R18" s="7"/>
-      <c r="S18" s="7"/>
-      <c r="T18" s="7"/>
-      <c r="U18" s="7"/>
-      <c r="V18" s="7"/>
-      <c r="W18" s="7"/>
-      <c r="X18" s="7"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+      <c r="U18" s="4"/>
+      <c r="V18" s="4"/>
+      <c r="W18" s="4"/>
+      <c r="X18" s="4"/>
     </row>
     <row r="19" spans="1:24" ht="20.100000000000001" customHeight="1">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7"/>
-      <c r="Q19" s="7"/>
-      <c r="R19" s="7"/>
-      <c r="S19" s="7"/>
-      <c r="T19" s="7"/>
-      <c r="U19" s="7"/>
-      <c r="V19" s="7"/>
-      <c r="W19" s="7"/>
-      <c r="X19" s="7"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4"/>
+      <c r="V19" s="4"/>
+      <c r="W19" s="4"/>
+      <c r="X19" s="4"/>
     </row>
     <row r="20" spans="1:24" ht="20.85" customHeight="1" thickBot="1">
-      <c r="A20" s="10">
+      <c r="A20" s="7">
         <v>1</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B20" s="8">
         <f>H20/G20</f>
-        <v>4619.1872508350561</v>
-      </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6">
-        <v>2.6369673616171299</v>
-      </c>
-      <c r="H20" s="6">
-        <v>12180.64601765</v>
-      </c>
-      <c r="I20" s="6"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="7"/>
-      <c r="S20" s="7"/>
-      <c r="T20" s="7"/>
-      <c r="U20" s="7"/>
-      <c r="V20" s="7"/>
-      <c r="W20" s="7"/>
-      <c r="X20" s="7"/>
+        <v>4614.490745481753</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3">
+        <v>2.63697646764478</v>
+      </c>
+      <c r="H20" s="3">
+        <v>12168.303506</v>
+      </c>
+      <c r="I20" s="3"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="4"/>
+      <c r="U20" s="4"/>
+      <c r="V20" s="4"/>
+      <c r="W20" s="4"/>
+      <c r="X20" s="4"/>
     </row>
     <row r="21" spans="1:24" ht="20.85" customHeight="1">
-      <c r="A21" s="37"/>
-      <c r="B21" s="37"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6">
-        <v>2.6369979810536202</v>
-      </c>
-      <c r="H21" s="6">
-        <v>12222.267742</v>
-      </c>
-      <c r="I21" s="6"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="7"/>
-      <c r="Q21" s="7"/>
-      <c r="R21" s="7"/>
-      <c r="S21" s="7"/>
-      <c r="T21" s="7"/>
-      <c r="U21" s="7"/>
-      <c r="V21" s="7"/>
-      <c r="W21" s="7"/>
-      <c r="X21" s="7"/>
+      <c r="A21" s="28"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3">
+        <v>2.6370071790613498</v>
+      </c>
+      <c r="H21" s="3">
+        <v>12209.800558000001</v>
+      </c>
+      <c r="I21" s="3"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
+      <c r="U21" s="4"/>
+      <c r="V21" s="4"/>
+      <c r="W21" s="4"/>
+      <c r="X21" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>